<commit_message>
Release plan and notes
</commit_message>
<xml_diff>
--- a/Project Management/Release/Release Plan/Release-Plan.xlsx
+++ b/Project Management/Release/Release Plan/Release-Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="0" windowWidth="21620" windowHeight="12200" tabRatio="500"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="24840" windowHeight="13720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Release Plan" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Features</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Current Student-My appointment</t>
   </si>
   <si>
-    <t>Edit Profile- Srudent/Staff</t>
-  </si>
-  <si>
     <t>Admin-Add/Update/Delete User</t>
   </si>
   <si>
@@ -54,7 +51,13 @@
     <t>Staff- My Appointment, with Accept and Reject and Mail</t>
   </si>
   <si>
-    <t>Release Date</t>
+    <t>Planned Release Date</t>
+  </si>
+  <si>
+    <t>Actual Release Date</t>
+  </si>
+  <si>
+    <t>Edit Profile- Student/Staff</t>
   </si>
 </sst>
 </file>
@@ -161,8 +164,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -198,11 +203,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,7 +542,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -543,10 +550,11 @@
     <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" style="1" customWidth="1"/>
-    <col min="4" max="9" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" ht="30">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -554,10 +562,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -567,15 +578,19 @@
       <c r="C2" s="4">
         <v>42458</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="4">
+        <v>42463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="30">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -585,15 +600,19 @@
       <c r="C4" s="6">
         <v>42464</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="6">
+        <v>42467</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -603,60 +622,69 @@
       <c r="C6" s="6">
         <v>42468</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30">
+      <c r="D6" s="6">
+        <v>42471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="9">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6">
         <v>42471</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="6">
+        <v>42475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11"/>
       <c r="C11"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="B12"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="B13"/>
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="B14"/>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="B15"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="B16"/>
       <c r="C16"/>
     </row>
@@ -697,7 +725,11 @@
       <c r="C25"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C9:C10"/>

</xml_diff>